<commit_message>
update excel for grant hist
</commit_message>
<xml_diff>
--- a/DataFiles_Excel/GrantHistoryBarChart/ACFgrantHistTable.xlsx
+++ b/DataFiles_Excel/GrantHistoryBarChart/ACFgrantHistTable.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jim.ide\Desktop\annual-report-html2excel\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ferris\Documents\TAGGS 2016 AR\TaggsAR2016-master\DataFiles_Excel\GrantHistoryBarChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5730"/>
   </bookViews>
   <sheets>
     <sheet name="ACFgrantHistTable" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,7 @@
     <t>ACF Award History</t>
   </si>
   <si>
-    <t>This table shows the grant awards and award dollars ACF made for FY 2011-2016. It is provided as a text alternative to the interactive chart on the ACF page of this website.</t>
-  </si>
-  <si>
     <t>ACF Grant Awards and Award Dollars Description</t>
-  </si>
-  <si>
-    <t>Grant awards and award dollars ACF made for FY 2011-2016.</t>
   </si>
   <si>
     <t>Fiscal Year</t>
@@ -40,6 +34,12 @@
   </si>
   <si>
     <t>Total Award Amount</t>
+  </si>
+  <si>
+    <t>This table shows the grant awards and award dollars ACF made for FY 2012-2016. It is provided as a text alternative to the interactive chart on the ACF page of this website.</t>
+  </si>
+  <si>
+    <t>Grant awards and award dollars ACF made for FY 2012-2016.</t>
   </si>
 </sst>
 </file>
@@ -910,7 +910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -926,7 +928,7 @@
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -934,7 +936,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -946,7 +948,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -958,13 +960,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>